<commit_message>
it's getting the correct filetypes
</commit_message>
<xml_diff>
--- a/queryOut.xlsx
+++ b/queryOut.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -379,53 +379,209 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Freeman</t>
+          <t>Methodist</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>misc/vb_byte.c.txt</t>
+          <t>misc/count_letters.txt</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">#include int main () unsigned int testdata[] {, }; const int num_testdata sizeof(testdata)/; unsigned int vbytes[sizeof(testdata)]; int num_vbytes unsigned int carry, onenum, onebyte, movebyte, nbits; int i; i=;  carry onenum &lt;  carry printf ("%.X ", carry + (onenum % ); vbytes [num_vbytes++] carry + (onenum %  ); onenum onenum &gt;&gt; /* shift right  bits, i.e. divide  */ printf ("\ndone encoding variable bytes, decode \n"); onenum nbits i=; &lt; num_vbytes; i++ onebyte vbytes[i]; printf ("%.X ", onebyte); movebyte (onebyte%) &lt;&lt; nbits; nbits += onenum onenum + movebyte; onebyte &gt;  /* carry set, end number */ printf (" decoded %d\n", onenum ); onenum nbits printf ("\ndone\n"); return </t>
+          <t xml:space="preserve">#include #include #include int main(int argc, char *argv[]) int letter[]; FILE *fin; int i; char onechar; &lt; i++ letter[i] fin fopen (argv[], "r"); (fin == NULL printf ("unable open file %s\n", argv[] ); exit(); (onechar getc(fin) != EOF isalpha(onechar) ++letter[tolower(onechar) 'a']; fclose (fin); &lt; i++ printf ("letter %c occurs %d times\n", + 'a', letter[i]); </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>misc/seo_email.txt</t>
+          <t>misc/count_letters_duplicate.txt</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">-----Original Message----- From: Atul Kumar [mailto:atul@outlook.com] Sent: Thursday, March  : AM Subject: First Page In Google $ Per Month Hi, My name Afsar Ali working reputed leading S.E.O. Company INDIA experience getting customer's websites top Google, Yahoo, Msn search engine rankings producing high revenue top page rank. Here We Have contract OR Bond . We provide S.E.O. Special Offer going following package. Monthly task Responsibilities:- .  Directory submissions .  Social Bookmaking Submissions .  classified submission . PDF Submisssion .  Deep Linking . PPT submission . Website testing suggestion .  One Way back links mix PR . Meta tags changes suggestions . Keyword research . Competitor Analysis . Heading tag changes . Alt tag changes . Interlinking wherever required. . Keyword Density site content. . HTML Site Map . XML site map Submission webmaster tool Best rates package are: USD  per month per project. Let know interested I would happy send details this. Kind Regards Afsar Ali Skype: snehadixit Whatsapp:+  Sent Outlook </t>
+          <t xml:space="preserve">#include #include #include int main(int argc, char *argv[]) int letter[]; FILE *fin; int i; char onechar; &lt; i++ letter[i] fin fopen (argv[], "r"); (fin == NULL printf ("unable open file %s\n", argv[] ); exit(); (onechar getc(fin) != EOF isalpha(onechar) ++letter[tolower(onechar) 'a']; fclose (fin); &lt; i++ printf ("letter %c occurs %d times\n", + 'a', letter[i]); </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>schedule.htm</t>
+          <t>textfiles/cow2.txt</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">SMU CS Spring  Schedule SMU CS Spring  Preliminary Schedule This page maintained latest schedule content activities. Date Topics Activity Jan Jan  Course overview, Introduction IR (chpt Hmwk  assigned, Reimaginging Search Jan Jan  Boolean Retrieval, Terms, Posting Lists (chpt Hmwk  assigned, Dark Web article, Mercator article Feb Feb  The Web crawling (chpt Hmwk  due Feb Feb  Scoring (vector space model) (chpt Hmwk  due, Hmwk  assigned, project  assigned, figure ., brown cow, cow  files, little lamb, textfiles Feb Feb  Wildcards spelling errors (chpt Levenshtein disance, soundex online Feb Feb  Indexing (chpt ), Index Compression (chpt Hmwk  due, Letter distribution, word morphing, Variable byte C program Mar Mar  Scoring (complete search model) (chpt Hmwk assigned, badfile Mar Mar  catch up, review, midterm Exam I Mar Mar  No class: Spring Break Example noindex page, text files Mar Mar  Evaluation information retrieval (chpt Hmwk  due, Project  due Mar Apr  Relevance feedback query expansion (chpt Hmwk  assigned, Project  assigned, co-occurence matrix exmple Apr Apr  Text Classification (chpt roadmap, SEO email, Bayes classifier, Poem classifier, football-hockey example, Apr Apr  Document Clustering (chpt Hmwk  due, Hmwk  assigned, Poem k-means kNN, hierarchical demo Apr Apr  Link Analysis (chpt The classics: Google PageRank HITS algorithm Apr Apr  Vector space classification (chpt Hmwk  due May  No class: Reading Day Project  due May Exam II, Take-home </t>
+          <t xml:space="preserve">How Brown Cow! </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
+          <t>http://www.wessa.net/rwasp_hierarchicalclustering.wasp</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Not Found Not Found The requested URL /~fmoore/http://www.wessa.net/rwasp_hierarchicalclustering.wasp found server. </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>misc/levenshtein.html</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Levenshtein Distance demo function LevenshteinDistance(a, b) var cost; var m a.length; var n b.length; // make sure a.length &gt;= b.length use O(min(n,m)) space (m &lt; n) var c a; b; b c; var o m; m n; n o; var r []; r[] []; (var c c &lt; n + ++c) r[][c] c; (var &lt; m + ++i) r[i] []; r[i][] i; var j j &lt; n + ++j cost a.charAt(  === b.charAt( j  ?  : r[i][j] minof( r[i-][j] + r[i][j-] + r[i-][j-] + cost ); return r[m][n]; function minof(x, y, z) (x &lt;= y &amp;&amp; x &lt;= z) return x; (y &lt;= x &amp;&amp; y &lt;= z) return y; return z; function do_calc() var s, s, len_s, len_s, dis; myform.distance.value ""; myform.string.value; myform.string.value; dis LevenshteinDistance( s, s); myform.distance.value dis; Levenshtein Distance calculator For example:FAST CATS  CATS DOGS  String : String : Distance </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>textfiles/cow4.txt</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brown cow. </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>dontgohere/bayes.html</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A simple naive bayes classifier implemented javascript Training section These four areas contained four canned paragraphs. Two Spanish two French. They used seed classifier (for two classifications). Alicia empezaba cansarse muy sentada junto su hermana en la orilla y de tener nada que hacer: una o dos veces ella habÃ­a mirÃ en el libro que estaba leyendo su hermana, pero tenÃ­a fotos o conversaciones en Ã©l, 'y Â¿quÃ© es el uso de un libro,' pensamiento Alicia 'sin imÃ¡genes o conversaciones?' Teach Spanish No habÃ­a nada tan muy notable en eso; ni lo hizo Alice creo que lo muy mucho hasta escuchar el conejo dice sÃ­ mismo, "Oh Estimado! Oh Estimado! Voy ser tarde!' (cuando ella pensÃ en luego, ocurriÃ ella que ella deberÃ­a han preguntado esto, pero al tiempo todo parecÃ­a absolutamente natural); pero cuando el conejo realmente tomÃ un reloj del bolsillo de su chaleco, y mirÃ y luego se apresurÃ en, Alice comenzÃ sus pies, para que brillÃ travÃ©s de su mente que nunca antes habÃ­a visto un conejo con un bolsillo de chaleco, o un reloj para sacar de ella, y quema con curiosidad, corriÃ por el campo despuÃ©s de que y por suerte fue justo tiempo para verlo pop abajo un agujero del conejo grande debajo del seto. Teach Spanish Alice commenÃ§ait Ã Ãªtre trÃ¨s fatiguÃ© d'Ãªtre assis par sa sÅur sur la rive et de n'avoir rien Ã faire : une ou deux fois elle avait regarda dans le livre que lisait sa soeur, mais il n'avait aucun photos ou des conversations en elle, Â« et quelle est l'utilitÃ© d'un livre, Â» pensa Alice "sans images ni conversations?" Teach French Il n'y avait rien de si trÃ¨s remarquables en ce que ni Alice le pense il trÃ¨s une grande partie de la route d'entendre le lapin dire Ã lui-mÃªme, Â« Oh cher ! Oh dear ! Je vais Ãªtre en retard! " (elle pensÃ© qu'il plus par la suite, elle s'est produite lors lui elle devait avez-vous demandÃ© Ã ce qu'au moment oÃ tout semblait tout Ã fait naturel) mais quand le lapin en fait eu une montre de sa poche de gilet, et le regarda et puis se prÃ©cipita sur, Alice commencÃ© Ã ses pieds, car il flashÃ© sur son esprit qu'elle n'avait jamais vu un lapin avec une poche de gilet, ou une montre pour qu'elle hors de lui, et gravure avec curiositÃ©, elle couru Ã travers le champ, aprÃ¨s qu'il et Ã©tÃ© heureusement juste Ã temps pour le voir pop dans un grand trou de lapin sous la haie. Teach French Here put training text classification. Sample Spanish: AsÃ­ ella fue pensando en su propia mente (asÃ­ como podÃ­a, para el dÃ­a caluroso la hacÃ­a sentir muy somnoliento y tonto), si el placer de hacer una cadena de Margarita es vale la pena levantarse y recoger las margaritas, cuando de pronto un conejo blanco con ojos rosados funcionaron cerca por ella. Sample French: Alors qu'elle examinait dans son propre esprit (ainsi qu'elle pu, pour la journÃ©e chaude lui fait sentir trÃ¨s somnolent et stupide), si le plaisir de faire une guirlande serait la peine de se lever et de ramasser les marguerites, quand tout Ã coup un lapin blanc aux yeux roses couru Ã©troite par elle. Spanish French Teach Guessing section Paste unseen text see well classifier does. Two samples guess: En otro momento abajo fue Alice despuÃ©s de Ã©l, ni una sola vez teniendo en cuenta cÃmo el mundo iba salir. Dans un autre moment bas suivit Alice, jamais vu comment elle Ã©tait dans le monde de sortir Ã nouveau. Guess The javascript code used perform bayesian analysis. Reference: http://www.dusbabek.org/~garyd/bayes/ </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>textfiles/index.html</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SMU CSE Spring  Textfiles Textfiles clustering golf  golf  golf  golf  golf  basketball  basketball  basketball  basketball  basketball  baseball  baseball  baseball  baseball  baseball  football  football  football  football  football  </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>http://www.gedpage.com/soundex.html</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Not Found Not Found The requested URL /~fmoore/http://www.gedpage.com/soundex.html found server. </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>misc/vb_byte.c.txt</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">#include int main () unsigned int testdata[] {, }; const int num_testdata sizeof(testdata)/; unsigned int vbytes[sizeof(testdata)]; int num_vbytes unsigned int carry, onenum, onebyte, movebyte, nbits; int i; i=;  carry onenum &lt;  carry printf ("%.X ", carry + (onenum % ); vbytes [num_vbytes++] carry + (onenum %  ); onenum onenum &gt;&gt; /* shift right  bits, i.e. divide  */ printf ("\ndone encoding variable bytes, decode \n"); onenum nbits i=; &lt; num_vbytes; i++ onebyte vbytes[i]; printf ("%.X ", onebyte); movebyte (onebyte%) &lt;&lt; nbits; nbits += onenum onenum + movebyte; onebyte &gt;  /* carry set, end number */ printf (" decoded %d\n", onenum ); onenum nbits printf ("\ndone\n"); return </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>dontgohere/bayes-poem.html</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A simple naive bayes classifier implemented javascript Training section These four areas contained four canned poems. Two Frost two Whitman. They used seed classifier (for two classifications). Now close windows hush fields: If trees must, let silently toss; No bird singing now, is, Be loss. It long ere marshes resume, I long ere earliest bird: So close windows hear wind, But see wind-stirred. Teach Frost- Thereâs patch old snow corner That I guessed Was blow-away paper rain Had brought rest. It speckled grime Small print overspread it, The news day Iâve forgottenâ If I ever read it. Teach Frost- Beginning studies first step pleasâd much, The mere fact consciousness, forms, power motion, The least insect animal, senses, eyesight, love, The first step I say awed pleasâd much, I hardly gone hardly wishâd go farther, But stop loiter time sing ecstatic songs. Teach Whitman- Lo, unbounded sea, On breast ship starting, spreading sails, carrying even moonsails. The pennant flying aloft speeds speeds stately- emulous waves press forward, They surround ship shining curving motions foam. Teach Whitman- Here put training text classification. Sample Frost: Some say world end fire, Some say ice. From Iâve tasted desire I hold favour fire. But perish twice, I think I know enough hate To say destruction ice Is also great And would suffice. Sample Whiteman: I dreamâd dream I saw city invincible attacks whole rest earth, I dreamâd new city Friends, Nothing greater quality robust love, led rest, It seen every hour actions men city, And looks words. Frost Whitman Teach Guessing section Paste unseen text see well classifier does. A sample guess: A plow, say, plow snow. They cannot mean plant it, noâ Unless bitterness mock At cultivated rock. Guess The javascript code used perform bayesian analysis. Reference: http://www.dusbabek.org/~garyd/bayes/ </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>textfiles/cow3.txt</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What cow brown cow? </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>index.htm</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freeman Moore SMU Spring  Spring  Freeman L. Moore, PhD email: fmoore@lyle.smu.edu Fall  CS Keep looking Course calendar latest information. Spring  T/Th : : pm Junkins   Syllabus  Syllabus The contents Web site sole responsibility Dr. Freeman Moore necessarily represent opinions policies Southern Methodist University. The administrator site Dr. Freeman Moore may contacted fmoore@lyle.smu.edu. </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>index_duplicate.htm</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Not Found Not Found The requested URL /~fmoore/index_duplicate.htm found server. </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>textfiles/cow1.txt</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How brown Brown Cow? </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>schedule.htm</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SMU CS Spring  Schedule SMU CS Spring  Preliminary Schedule This page maintained latest schedule content activities. Date Topics Activity Jan Jan  Course overview, Introduction IR (chpt Hmwk  assigned, Reimaginging Search Jan Jan  Boolean Retrieval, Terms, Posting Lists (chpt Hmwk  assigned, Dark Web article, Mercator article Feb Feb  The Web crawling (chpt Hmwk  due Feb Feb  Scoring (vector space model) (chpt Hmwk  due, Hmwk  assigned, project  assigned, figure ., brown cow, cow  files, little lamb, textfiles Feb Feb  Wildcards spelling errors (chpt Levenshtein disance, soundex online Feb Feb  Indexing (chpt ), Index Compression (chpt Hmwk  due, Letter distribution, word morphing, Variable byte C program Mar Mar  Scoring (complete search model) (chpt Hmwk assigned, badfile Mar Mar  catch up, review, midterm Exam I Mar Mar  No class: Spring Break Example noindex page, text files Mar Mar  Evaluation information retrieval (chpt Hmwk  due, Project  due Mar Apr  Relevance feedback query expansion (chpt Hmwk  assigned, Project  assigned, co-occurence matrix exmple Apr Apr  Text Classification (chpt roadmap, SEO email, Bayes classifier, Poem classifier, football-hockey example, Apr Apr  Document Clustering (chpt Hmwk  due, Hmwk  assigned, Poem k-means kNN, hierarchical demo Apr Apr  Link Analysis (chpt The classics: Google PageRank HITS algorithm Apr Apr  Vector space classification (chpt Hmwk  due May  No class: Reading Day Project  due May Exam II, Take-home </t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
           <t>placeholder</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>this is to start dataframe</t>
         </is>

</xml_diff>